<commit_message>
started results for heston_sl on zynq
</commit_message>
<xml_diff>
--- a/results/2013.08.30_heston_sl_laptop/results.xlsx
+++ b/results/2013.08.30_heston_sl_laptop/results.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="3960" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Heston SL: run_cpu.cpp</t>
   </si>
@@ -25,12 +25,6 @@
     <t>Compiled with 32 bit</t>
   </si>
   <si>
-    <t>557568 values / sec</t>
-  </si>
-  <si>
-    <t>35.5 Watt</t>
-  </si>
-  <si>
     <t>Compiler:</t>
   </si>
   <si>
@@ -82,10 +76,19 @@
     <t>4 Threads</t>
   </si>
   <si>
-    <t>= 139.4e6 steps / sec</t>
-  </si>
-  <si>
-    <t>= 255 nJ / step</t>
+    <t>values / sec</t>
+  </si>
+  <si>
+    <t>steps / sec</t>
+  </si>
+  <si>
+    <t>Watt</t>
+  </si>
+  <si>
+    <t>J / step</t>
+  </si>
+  <si>
+    <t>Power Efficiency:</t>
   </si>
 </sst>
 </file>
@@ -129,13 +132,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -151,9 +155,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -191,7 +195,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -263,7 +267,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -437,11 +441,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -450,32 +459,32 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -490,78 +499,103 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>557568</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <f>A23*250</f>
+        <v>139392000</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>35.5</v>
+      </c>
+      <c r="B27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <f>A27/A24</f>
+        <v>2.5467745638200184E-7</v>
+      </c>
+      <c r="B31" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new pwer meter laptop & date comparison
</commit_message>
<xml_diff>
--- a/results/2013.08.30_heston_sl_laptop/results.xlsx
+++ b/results/2013.08.30_heston_sl_laptop/results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Heston SL: run_cpu.cpp</t>
   </si>
@@ -106,14 +106,20 @@
     <t>Power (Volcraft VC 870, run_cpu)</t>
   </si>
   <si>
-    <t xml:space="preserve">Version: </t>
+    <t>Version: 22425123e417c44fe57514d14b7c0cf6c4ca185b</t>
+  </si>
+  <si>
+    <t>Performance (run_cpu):</t>
+  </si>
+  <si>
+    <t>Display aus, Batterie raus, Netwerk aus, Wifi aus, Reboot &amp; Warmup, Multiple starts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +131,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -150,12 +171,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="48" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="48" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -460,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,111 +583,142 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="25" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
         <v>557568</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
-        <f>A24*250</f>
+    <row r="26" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <f>A25*250</f>
         <v>139392000</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+    </row>
+    <row r="28" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="29" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
         <v>35.5</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <f>A28/A25</f>
+    <row r="33" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <f>A29/A26</f>
         <v>2.5467745638200184E-7</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>141086000</v>
+      </c>
+      <c r="B38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>23</v>
       </c>
-      <c r="C37">
+      <c r="C41">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>22</v>
       </c>
-      <c r="C38">
+      <c r="C42">
         <v>12.9</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>24</v>
       </c>
-      <c r="C39">
+      <c r="C43">
         <v>11.2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>25</v>
       </c>
-      <c r="C40">
+      <c r="C44">
         <v>30.6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <f>C44/A38</f>
+        <v>2.1688898969422907E-7</v>
+      </c>
+      <c r="B47" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>